<commit_message>
saving changes to postProcessing.R
</commit_message>
<xml_diff>
--- a/ldaresults_test_set_sorted_curatedafg_100.xlsx
+++ b/ldaresults_test_set_sorted_curatedafg_100.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>x</t>
   </si>
@@ -20,28 +20,142 @@
     <t>3</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>13</t>
   </si>
   <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
     <t>37</t>
   </si>
   <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
     <t>48</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
+    <t>25</t>
+  </si>
+  <si>
+    <t>38</t>
   </si>
   <si>
     <t>7</t>
@@ -50,124 +164,7 @@
     <t>8</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>51</t>
   </si>
 </sst>
 </file>
@@ -237,7 +234,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
@@ -261,7 +258,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="7">
@@ -277,7 +274,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="9">
@@ -285,7 +282,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="10">
@@ -293,7 +290,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="11">
@@ -301,7 +298,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="12">
@@ -333,7 +330,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="16">
@@ -349,7 +346,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="18">
@@ -357,7 +354,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="19">
@@ -373,7 +370,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="21">
@@ -397,7 +394,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="24">
@@ -413,7 +410,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="26">
@@ -429,7 +426,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="28">
@@ -437,7 +434,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="29">
@@ -485,7 +482,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="35">
@@ -501,7 +498,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="37">
@@ -509,7 +506,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="38">
@@ -517,7 +514,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="39">
@@ -525,7 +522,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="40">
@@ -541,7 +538,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="42">
@@ -549,7 +546,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="43">
@@ -557,7 +554,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="44">
@@ -565,7 +562,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="45">
@@ -581,7 +578,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="47">
@@ -589,7 +586,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="48">
@@ -597,7 +594,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="49">
@@ -621,15 +618,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s">
-        <v>51</v>
-      </c>
-      <c r="B52" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
preliminary charts added for final paper, bug in creating confusion matrix fixed
</commit_message>
<xml_diff>
--- a/ldaresults_test_set_sorted_curatedafg_100.xlsx
+++ b/ldaresults_test_set_sorted_curatedafg_100.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>x</t>
   </si>
@@ -20,76 +20,226 @@
     <t>1</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>5</t>
   </si>
   <si>
+    <t>7</t>
+  </si>
+  <si>
     <t>10</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>21</t>
+    <t>11</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
   <si>
     <t>25</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>14</t>
   </si>
 </sst>
 </file>
@@ -151,7 +301,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="3">
@@ -175,7 +325,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="6">
@@ -183,7 +333,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="7">
@@ -199,7 +349,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="9">
@@ -207,7 +357,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="10">
@@ -215,7 +365,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="11">
@@ -223,7 +373,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="12">
@@ -247,7 +397,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="15">
@@ -255,7 +405,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="16">
@@ -263,7 +413,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="17">
@@ -271,7 +421,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="18">
@@ -279,7 +429,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="19">
@@ -287,7 +437,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="20">
@@ -295,7 +445,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="21">
@@ -303,7 +453,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="22">
@@ -311,7 +461,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="23">
@@ -319,7 +469,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="24">
@@ -327,7 +477,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="25">
@@ -335,7 +485,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="26">
@@ -343,7 +493,407 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" t="n">
         <v>2.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+      <c r="B73" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>73</v>
+      </c>
+      <c r="B74" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76" t="n">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>